<commit_message>
Update - Aula 00 and Aula 01
New files of Aula 01 and updated files for Aula 00.
</commit_message>
<xml_diff>
--- a/motocicletas.xlsx
+++ b/motocicletas.xlsx
@@ -5,19 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Le Bomb\kgalois\FMU\2022.2\2022.2-fmu-estatistica-avancada\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Le Bomb\kgalois\FMU\2022.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4048DF-E666-4E5A-A24F-D1CD92B99568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4ECC8DD-E299-4A9E-80DE-2D0E5C1B8D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D1CACCC8-E1BD-4E6E-BE0A-384E465C6131}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1CACCC8-E1BD-4E6E-BE0A-384E465C6131}"/>
   </bookViews>
   <sheets>
     <sheet name="motocicletas" sheetId="1" r:id="rId1"/>
-    <sheet name="analise-descritiva-D" sheetId="2" r:id="rId2"/>
-    <sheet name="graficos-D" sheetId="3" r:id="rId3"/>
-    <sheet name="analise-descritiva-N" sheetId="4" r:id="rId4"/>
-    <sheet name="graficos-N" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -264,7 +260,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -275,6 +290,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AEAD4907-8B44-4E2D-AC3E-6E996A1A6C9F}" name="Tabela1" displayName="Tabela1" ref="A1:I37" totalsRowShown="0">
+  <autoFilter ref="A1:I37" xr:uid="{AEAD4907-8B44-4E2D-AC3E-6E996A1A6C9F}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{3A309B3E-4BD4-4670-B3F0-EE7079B6E0CC}" name="Nome"/>
+    <tableColumn id="2" xr3:uid="{14239AA3-4D9D-45B6-9D79-3D19A1C9483A}" name="Marca" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{64820868-2BFB-4608-A7A3-4E9AF955CB21}" name="Modelo"/>
+    <tableColumn id="4" xr3:uid="{0030761B-3AE6-4F8C-8295-84C30DA03459}" name="Preço"/>
+    <tableColumn id="5" xr3:uid="{62B125BD-4BAB-43BC-8DD6-2C5C102E176E}" name="Cilindradas"/>
+    <tableColumn id="6" xr3:uid="{B49FFC55-108E-421F-AB20-1FBF97ECCCB4}" name="Capacidade (L)"/>
+    <tableColumn id="7" xr3:uid="{EBC05C77-C7A8-49B6-9EA0-CE632EBDD5AE}" name="Combustível"/>
+    <tableColumn id="8" xr3:uid="{FDC84B30-8469-4785-A9CB-1153513E1719}" name="Tipo de Freio"/>
+    <tableColumn id="9" xr3:uid="{490E63A9-4206-47C6-99D3-B4E74AB22FAA}" name="Peso Seco da Moto (kg)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -576,18 +609,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE497D9-27E2-4EA7-A792-B04431AC1CBB}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1233,6 +1267,7 @@
       <c r="I22">
         <v>153</v>
       </c>
+      <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1685,57 +1720,8 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2254791-6A82-4DC6-B1AC-7A904B218F9F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136664C9-652D-49BF-BB65-BE9A2C413D9F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E5B771-B695-4E4F-91BE-9A9E364C618F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB8243A-698A-4066-A7DC-CC462C9842D8}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>